<commit_message>
Fixed The Sprint Backlog
Added more tasks.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog  Burndown.xlsx
+++ b/documentation/Sprint Backlog  Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gn00021\Desktop\SoftwareEngineering_Project1\SoftwareEngineeringProject1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40BA041-DDC4-46ED-B49B-66C9339CE7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AFBEE5-950D-40D8-B1A2-0B18A2CC0DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Related User Story</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Day 4</t>
+  </si>
+  <si>
+    <t>Require compartment to be selected</t>
   </si>
 </sst>
 </file>
@@ -209,6 +212,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC0C0C0"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -312,12 +320,12 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$26:$G$26</c:f>
+              <c:f>Sheet1!$C$27:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1073,13 +1081,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>93662</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>138112</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>112712</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1371,10 +1379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,46 +1433,46 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -1474,7 +1482,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1482,17 +1490,17 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1500,43 +1508,43 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
@@ -1546,25 +1554,25 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1572,28 +1580,36 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -1726,31 +1742,41 @@
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="3">
-        <f>SUM(C3:C25)</f>
-        <v>22</v>
-      </c>
-      <c r="D26" s="3">
-        <f>SUM(D3:D25)</f>
+      <c r="C27" s="3">
+        <f>SUM(C4:C26)</f>
+        <v>31</v>
+      </c>
+      <c r="D27" s="3">
+        <f>SUM(D4:D26)</f>
         <v>0</v>
       </c>
-      <c r="E26" s="3">
-        <f>SUM(E3:E25)</f>
+      <c r="E27" s="3">
+        <f>SUM(E4:E26)</f>
         <v>0</v>
       </c>
-      <c r="F26" s="3">
-        <f>SUM(F3:F25)</f>
+      <c r="F27" s="3">
+        <f>SUM(F4:F26)</f>
         <v>0</v>
       </c>
-      <c r="G26" s="3">
-        <f>SUM(G3:G25)</f>
+      <c r="G27" s="3">
+        <f>SUM(G4:G26)</f>
         <v>0</v>
       </c>
-      <c r="H26" s="3">
-        <f>SUM(H3:H25)</f>
+      <c r="H27" s="3">
+        <f>SUM(H4:H26)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a password field
i added a password field to replace the text field in the login page this in turn makes the system feel more secure
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog  Burndown.xlsx
+++ b/documentation/Sprint Backlog  Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gn00021\Desktop\SoftwareEngineering_Project1\SoftwareEngineeringProject1\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jr00381\Desktop\SE1 GROUP PROJCET\SoftwareEngineeringProject1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AFBEE5-950D-40D8-B1A2-0B18A2CC0DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F276204F-A07C-4472-B148-78CEE1DFCDB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -328,10 +328,10 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1382,7 +1382,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,8 +1513,12 @@
       <c r="C7" s="1">
         <v>5</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="1" t="s">
@@ -1585,9 +1589,15 @@
       <c r="C11" s="1">
         <v>3</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="1" t="s">
         <v>20</v>
@@ -1756,27 +1766,27 @@
         <v>4</v>
       </c>
       <c r="C27" s="3">
-        <f>SUM(C4:C26)</f>
+        <f t="shared" ref="C27:H27" si="0">SUM(C4:C26)</f>
         <v>31</v>
       </c>
       <c r="D27" s="3">
-        <f>SUM(D4:D26)</f>
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F27" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="3">
-        <f>SUM(E4:E26)</f>
+      <c r="G27" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F27" s="3">
-        <f>SUM(F4:F26)</f>
-        <v>0</v>
-      </c>
-      <c r="G27" s="3">
-        <f>SUM(G4:G26)</f>
-        <v>0</v>
-      </c>
       <c r="H27" s="3">
-        <f>SUM(H4:H26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Sprint Backlog Hours
Updated my task completion hours
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog  Burndown.xlsx
+++ b/documentation/Sprint Backlog  Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jr00381\Desktop\SE1 GROUP PROJCET\SoftwareEngineeringProject1\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gn00021\Desktop\SoftwareEngineering_Project1\SoftwareEngineeringProject1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F276204F-A07C-4472-B148-78CEE1DFCDB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610D3105-D27C-4494-B025-556048D99BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="9945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -206,6 +206,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -328,10 +329,10 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1382,7 +1383,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1441,8 +1442,12 @@
       <c r="C3" s="1">
         <v>4</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="D3" s="8">
+        <v>4</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
+      </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="1" t="s">
@@ -1495,9 +1500,15 @@
       <c r="C6" s="1">
         <v>3</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="D6" s="2">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="1" t="s">
         <v>19</v>
@@ -1771,11 +1782,11 @@
       </c>
       <c r="D27" s="3">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Edited Sprint Backlog Hours
Edited hours for my tasks for the burndown.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog  Burndown.xlsx
+++ b/documentation/Sprint Backlog  Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jr00381\Desktop\SE1 GROUP PROJCET\SoftwareEngineeringProject1\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js00547\Documents\SOFTWARE ENGINEERING\SoftwareEngineeringProject1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F276204F-A07C-4472-B148-78CEE1DFCDB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C49E982-617B-4793-9AF7-9654A2F0B513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -328,13 +328,13 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1382,18 +1382,18 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1477,7 +1477,9 @@
       <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1485,7 +1487,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1503,7 +1505,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1525,7 +1527,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1535,15 +1537,23 @@
       <c r="C8" s="1">
         <v>5</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="D8" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
       <c r="H8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1561,7 +1571,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1579,7 +1589,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1603,7 +1613,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1621,7 +1631,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1631,7 +1641,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1641,7 +1651,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1651,7 +1661,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1661,7 +1671,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1671,7 +1681,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1681,7 +1691,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1691,7 +1701,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1701,7 +1711,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1711,7 +1721,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1721,7 +1731,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1731,7 +1741,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1741,7 +1751,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1751,7 +1761,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1761,7 +1771,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
         <v>4</v>
       </c>
@@ -1771,15 +1781,15 @@
       </c>
       <c r="D27" s="3">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12.5</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>7.5</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G27" s="3">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Added Remove Stock Button Functionality
Added the button and functionality to it.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog  Burndown.xlsx
+++ b/documentation/Sprint Backlog  Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gn00021\Desktop\SoftwareEngineering_Project1\SoftwareEngineeringProject1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610D3105-D27C-4494-B025-556048D99BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502E79C0-71F3-41A9-9334-1C1D513A2330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="9945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="555" windowWidth="22950" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -200,6 +200,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -329,13 +330,13 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1383,7 +1384,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,29 +1396,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="7" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="5" t="s">
         <v>23</v>
       </c>
@@ -1430,7 +1431,7 @@
       <c r="G2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="7"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1442,14 +1443,18 @@
       <c r="C3" s="1">
         <v>4</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="6">
         <v>4</v>
       </c>
-      <c r="E3" s="8">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9">
+        <v>0</v>
+      </c>
       <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1464,10 +1469,18 @@
       <c r="C4" s="1">
         <v>3</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="D4" s="2">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
       <c r="H4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1482,10 +1495,18 @@
       <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
       <c r="H5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1509,7 +1530,9 @@
       <c r="F6" s="2">
         <v>0</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
       <c r="H6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1530,8 +1553,12 @@
       <c r="E7" s="2">
         <v>0</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
       <c r="H7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1546,10 +1573,18 @@
       <c r="C8" s="1">
         <v>5</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
       <c r="H8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1564,10 +1599,18 @@
       <c r="C9" s="1">
         <v>3</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
       <c r="H9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1582,10 +1625,18 @@
       <c r="C10" s="1">
         <v>4</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="D10" s="2">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
       <c r="H10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1609,7 +1660,9 @@
       <c r="F11" s="2">
         <v>0</v>
       </c>
-      <c r="G11" s="2"/>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
       <c r="H11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1624,10 +1677,18 @@
       <c r="C12" s="1">
         <v>3</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="D12" s="2">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
       <c r="H12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1782,15 +1843,15 @@
       </c>
       <c r="D27" s="3">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G27" s="3">
         <f t="shared" si="0"/>

</xml_diff>